<commit_message>
Remove Bin and Obj folders
</commit_message>
<xml_diff>
--- a/PatientMgmtSystemTestsResults/Failed - T4000_Newly_created_hospital_displays_on_hospital_list.xlsx
+++ b/PatientMgmtSystemTestsResults/Failed - T4000_Newly_created_hospital_displays_on_hospital_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16608" windowHeight="9432"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -651,19 +651,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:123" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:123" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>15</v>
       </c>
@@ -677,7 +677,7 @@
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:123" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -685,7 +685,7 @@
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
     </row>
-    <row r="3" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,7 +699,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:123" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -713,7 +713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:123" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -727,13 +727,13 @@
         <v>41961</v>
       </c>
     </row>
-    <row r="6" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:123" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:123" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>5</v>
       </c>
@@ -745,7 +745,7 @@
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>20</v>
       </c>
@@ -757,7 +757,7 @@
       <c r="G8" s="21"/>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -767,7 +767,7 @@
       <c r="G9" s="21"/>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:123" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -777,7 +777,7 @@
       <c r="G10" s="21"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:123" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:123" ht="110.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -787,7 +787,7 @@
       <c r="G11" s="21"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="1:123" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:123" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -796,7 +796,7 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:123" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:123" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>6</v>
       </c>
@@ -937,7 +937,7 @@
       <c r="DR13" s="12"/>
       <c r="DS13" s="12"/>
     </row>
-    <row r="14" spans="1:123" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:123" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -1067,7 +1067,7 @@
       <c r="DR14" s="13"/>
       <c r="DS14" s="13"/>
     </row>
-    <row r="15" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>20</v>
       </c>
@@ -1197,7 +1197,7 @@
       <c r="DR15" s="13"/>
       <c r="DS15" s="13"/>
     </row>
-    <row r="16" spans="1:123" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:123" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>30</v>
       </c>
@@ -1330,7 +1330,7 @@
       <c r="DR16" s="13"/>
       <c r="DS16" s="13"/>
     </row>
-    <row r="17" spans="1:123" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:123" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>40</v>
       </c>
@@ -1463,7 +1463,7 @@
       <c r="DR17" s="13"/>
       <c r="DS17" s="13"/>
     </row>
-    <row r="18" spans="1:123" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:123" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>50</v>
       </c>
@@ -1596,7 +1596,7 @@
       <c r="DR18" s="13"/>
       <c r="DS18" s="13"/>
     </row>
-    <row r="19" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H19" s="11"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
@@ -1714,7 +1714,7 @@
       <c r="DR19" s="13"/>
       <c r="DS19" s="13"/>
     </row>
-    <row r="20" spans="1:123" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:123" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H20" s="7"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
@@ -1832,7 +1832,7 @@
       <c r="DR20" s="13"/>
       <c r="DS20" s="13"/>
     </row>
-    <row r="21" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H21" s="11"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
@@ -1950,7 +1950,7 @@
       <c r="DR21" s="13"/>
       <c r="DS21" s="13"/>
     </row>
-    <row r="22" spans="1:123" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:123" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H22" s="7"/>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
@@ -2068,7 +2068,7 @@
       <c r="DR22" s="13"/>
       <c r="DS22" s="13"/>
     </row>
-    <row r="23" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H23" s="11"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
@@ -2186,7 +2186,7 @@
       <c r="DR23" s="13"/>
       <c r="DS23" s="13"/>
     </row>
-    <row r="24" spans="1:123" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:123" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H24" s="7"/>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
@@ -2304,7 +2304,7 @@
       <c r="DR24" s="13"/>
       <c r="DS24" s="13"/>
     </row>
-    <row r="25" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H25" s="11"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -2422,7 +2422,7 @@
       <c r="DR25" s="13"/>
       <c r="DS25" s="13"/>
     </row>
-    <row r="26" spans="1:123" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:123" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H26" s="7"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
@@ -2540,7 +2540,7 @@
       <c r="DR26" s="13"/>
       <c r="DS26" s="13"/>
     </row>
-    <row r="27" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H27" s="11"/>
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
@@ -2658,7 +2658,7 @@
       <c r="DR27" s="13"/>
       <c r="DS27" s="13"/>
     </row>
-    <row r="28" spans="1:123" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:123" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H28" s="7"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
@@ -2776,7 +2776,7 @@
       <c r="DR28" s="13"/>
       <c r="DS28" s="13"/>
     </row>
-    <row r="29" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:123" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H29" s="11"/>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
@@ -2894,16 +2894,16 @@
       <c r="DR29" s="13"/>
       <c r="DS29" s="13"/>
     </row>
-    <row r="30" spans="1:123" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:123" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:123" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:123" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:123" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:123" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2912,7 +2912,7 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>

</xml_diff>